<commit_message>
added function to name Unnamed columns, next remove code to unhandle unnamed columns
</commit_message>
<xml_diff>
--- a/Leerplanillacupos/data/030323.xlsx
+++ b/Leerplanillacupos/data/030323.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gastonmousques/workspace/ExcelExporter/excelconverter/Leerplanillacupos/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\workspace\excelconverter\Leerplanillacupos\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7ED3858-F36D-D54C-B1D4-DDBBBF052EB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F17DE59-37F8-47E8-A11B-BECE6ED60872}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="80" yWindow="760" windowWidth="30160" windowHeight="18880" xr2:uid="{E2EAB03B-CC58-F343-82B4-968B67AFF3DB}"/>
+    <workbookView xWindow="28680" yWindow="1830" windowWidth="24240" windowHeight="13140" xr2:uid="{E2EAB03B-CC58-F343-82B4-968B67AFF3DB}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1476" uniqueCount="702">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1475" uniqueCount="701">
   <si>
     <t>Id</t>
   </si>
@@ -2133,9 +2133,6 @@
   </si>
   <si>
     <t xml:space="preserve"> Calidad de software</t>
-  </si>
-  <si>
-    <t>fecha</t>
   </si>
   <si>
     <t>Ins_Cupo</t>
@@ -2145,7 +2142,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -2230,7 +2227,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -2254,7 +2251,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2273,7 +2269,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - Tema de 2022">
   <a:themeElements>
     <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
@@ -2569,24 +2565,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB01C85B-E3F0-6643-87D6-9914D08D3EBF}">
-  <dimension ref="A1:H302"/>
+  <dimension ref="B1:H302"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="27.19921875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="35.19921875" customWidth="1"/>
-    <col min="7" max="7" width="17.796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="35.140625" customWidth="1"/>
+    <col min="7" max="7" width="17.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
-      <c r="A1" t="s">
-        <v>700</v>
-      </c>
+    <row r="1" spans="2:8" ht="13.5" x14ac:dyDescent="0.2">
       <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
@@ -2604,13 +2597,10 @@
         <v>4</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>701</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8">
-      <c r="A2" s="9">
-        <v>44988</v>
-      </c>
+        <v>700</v>
+      </c>
+    </row>
+    <row r="2" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B2" s="6">
         <v>64137</v>
       </c>
@@ -2631,10 +2621,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
-      <c r="A3" s="9">
-        <v>44988</v>
-      </c>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B3" s="6">
         <v>64141</v>
       </c>
@@ -2657,10 +2644,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
-      <c r="A4" s="9">
-        <v>44988</v>
-      </c>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B4" s="6">
         <v>64171</v>
       </c>
@@ -2683,10 +2667,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
-      <c r="A5" s="9">
-        <v>44988</v>
-      </c>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B5" s="6">
         <v>64609</v>
       </c>
@@ -2709,10 +2690,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
-      <c r="A6" s="9">
-        <v>44988</v>
-      </c>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B6" s="6">
         <v>64610</v>
       </c>
@@ -2735,10 +2713,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
-      <c r="A7" s="9">
-        <v>44988</v>
-      </c>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B7" s="6">
         <v>64611</v>
       </c>
@@ -2761,10 +2736,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
-      <c r="A8" s="9">
-        <v>44988</v>
-      </c>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B8" s="6">
         <v>64612</v>
       </c>
@@ -2787,10 +2759,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
-      <c r="A9" s="9">
-        <v>44988</v>
-      </c>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B9" s="6">
         <v>65510</v>
       </c>
@@ -2813,10 +2782,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
-      <c r="A10" s="9">
-        <v>44988</v>
-      </c>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B10" s="6">
         <v>65555</v>
       </c>
@@ -2839,10 +2805,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
-      <c r="A11" s="9">
-        <v>44988</v>
-      </c>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B11" s="6">
         <v>64806</v>
       </c>
@@ -2865,10 +2828,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
-      <c r="A12" s="9">
-        <v>44988</v>
-      </c>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B12" s="6">
         <v>65134</v>
       </c>
@@ -2891,10 +2851,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
-      <c r="A13" s="9">
-        <v>44988</v>
-      </c>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B13" s="6">
         <v>64201</v>
       </c>
@@ -2917,10 +2874,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
-      <c r="A14" s="9">
-        <v>44988</v>
-      </c>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B14" s="6">
         <v>64205</v>
       </c>
@@ -2943,10 +2897,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
-      <c r="A15" s="9">
-        <v>44988</v>
-      </c>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B15" s="6">
         <v>64209</v>
       </c>
@@ -2969,10 +2920,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
-      <c r="A16" s="9">
-        <v>44988</v>
-      </c>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B16" s="6">
         <v>64213</v>
       </c>
@@ -2995,10 +2943,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="17" spans="1:8">
-      <c r="A17" s="9">
-        <v>44988</v>
-      </c>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B17" s="6">
         <v>64217</v>
       </c>
@@ -3021,10 +2966,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="18" spans="1:8">
-      <c r="A18" s="9">
-        <v>44988</v>
-      </c>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B18" s="6">
         <v>64221</v>
       </c>
@@ -3047,10 +2989,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="19" spans="1:8">
-      <c r="A19" s="9">
-        <v>44988</v>
-      </c>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B19" s="6">
         <v>64226</v>
       </c>
@@ -3073,10 +3012,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="20" spans="1:8">
-      <c r="A20" s="9">
-        <v>44988</v>
-      </c>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B20" s="6">
         <v>64230</v>
       </c>
@@ -3099,10 +3035,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="21" spans="1:8">
-      <c r="A21" s="9">
-        <v>44988</v>
-      </c>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B21" s="6">
         <v>64235</v>
       </c>
@@ -3125,10 +3058,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="22" spans="1:8">
-      <c r="A22" s="9">
-        <v>44988</v>
-      </c>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B22" s="6">
         <v>64306</v>
       </c>
@@ -3151,10 +3081,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="23" spans="1:8">
-      <c r="A23" s="9">
-        <v>44988</v>
-      </c>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B23" s="6">
         <v>64455</v>
       </c>
@@ -3177,10 +3104,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="24" spans="1:8">
-      <c r="A24" s="9">
-        <v>44988</v>
-      </c>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B24" s="6">
         <v>64754</v>
       </c>
@@ -3201,10 +3125,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="25" spans="1:8">
-      <c r="A25" s="9">
-        <v>44988</v>
-      </c>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B25" s="6">
         <v>64166</v>
       </c>
@@ -3227,10 +3148,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="26" spans="1:8">
-      <c r="A26" s="9">
-        <v>44988</v>
-      </c>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B26" s="6">
         <v>64186</v>
       </c>
@@ -3253,10 +3171,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="27" spans="1:8">
-      <c r="A27" s="9">
-        <v>44988</v>
-      </c>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B27" s="6">
         <v>64804</v>
       </c>
@@ -3279,10 +3194,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="28" spans="1:8">
-      <c r="A28" s="9">
-        <v>44988</v>
-      </c>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B28" s="6">
         <v>64337</v>
       </c>
@@ -3305,10 +3217,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="29" spans="1:8">
-      <c r="A29" s="9">
-        <v>44988</v>
-      </c>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B29" s="6">
         <v>65188</v>
       </c>
@@ -3331,10 +3240,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="30" spans="1:8">
-      <c r="A30" s="9">
-        <v>44988</v>
-      </c>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B30" s="6">
         <v>64252</v>
       </c>
@@ -3357,10 +3263,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="31" spans="1:8">
-      <c r="A31" s="9">
-        <v>44988</v>
-      </c>
+    <row r="31" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B31" s="6">
         <v>64256</v>
       </c>
@@ -3383,10 +3286,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="32" spans="1:8">
-      <c r="A32" s="9">
-        <v>44988</v>
-      </c>
+    <row r="32" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B32" s="6">
         <v>64260</v>
       </c>
@@ -3409,10 +3309,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="33" spans="1:8">
-      <c r="A33" s="9">
-        <v>44988</v>
-      </c>
+    <row r="33" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B33" s="6">
         <v>64264</v>
       </c>
@@ -3435,10 +3332,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="34" spans="1:8">
-      <c r="A34" s="9">
-        <v>44988</v>
-      </c>
+    <row r="34" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B34" s="6">
         <v>64313</v>
       </c>
@@ -3461,10 +3355,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="35" spans="1:8">
-      <c r="A35" s="9">
-        <v>44988</v>
-      </c>
+    <row r="35" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B35" s="6">
         <v>64292</v>
       </c>
@@ -3487,10 +3378,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="36" spans="1:8">
-      <c r="A36" s="9">
-        <v>44988</v>
-      </c>
+    <row r="36" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B36" s="6">
         <v>64328</v>
       </c>
@@ -3513,10 +3401,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="37" spans="1:8">
-      <c r="A37" s="9">
-        <v>44988</v>
-      </c>
+    <row r="37" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B37" s="6">
         <v>64332</v>
       </c>
@@ -3539,10 +3424,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="38" spans="1:8">
-      <c r="A38" s="9">
-        <v>44988</v>
-      </c>
+    <row r="38" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B38" s="6">
         <v>64194</v>
       </c>
@@ -3565,10 +3447,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="39" spans="1:8">
-      <c r="A39" s="9">
-        <v>44988</v>
-      </c>
+    <row r="39" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B39" s="6">
         <v>65150</v>
       </c>
@@ -3591,10 +3470,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="40" spans="1:8">
-      <c r="A40" s="9">
-        <v>44988</v>
-      </c>
+    <row r="40" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B40" s="6">
         <v>64301</v>
       </c>
@@ -3617,10 +3493,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="41" spans="1:8">
-      <c r="A41" s="9">
-        <v>44988</v>
-      </c>
+    <row r="41" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B41" s="6">
         <v>64331</v>
       </c>
@@ -3643,10 +3516,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="42" spans="1:8">
-      <c r="A42" s="9">
-        <v>44988</v>
-      </c>
+    <row r="42" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B42" s="6">
         <v>64336</v>
       </c>
@@ -3669,10 +3539,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="43" spans="1:8">
-      <c r="A43" s="9">
-        <v>44988</v>
-      </c>
+    <row r="43" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B43" s="6">
         <v>64149</v>
       </c>
@@ -3695,10 +3562,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="44" spans="1:8">
-      <c r="A44" s="9">
-        <v>44988</v>
-      </c>
+    <row r="44" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B44" s="6">
         <v>64153</v>
       </c>
@@ -3721,10 +3585,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="45" spans="1:8">
-      <c r="A45" s="9">
-        <v>44988</v>
-      </c>
+    <row r="45" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B45" s="6">
         <v>64176</v>
       </c>
@@ -3747,10 +3608,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="46" spans="1:8">
-      <c r="A46" s="9">
-        <v>44988</v>
-      </c>
+    <row r="46" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B46" s="6">
         <v>64268</v>
       </c>
@@ -3773,10 +3631,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="47" spans="1:8">
-      <c r="A47" s="9">
-        <v>44988</v>
-      </c>
+    <row r="47" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B47" s="6">
         <v>64272</v>
       </c>
@@ -3799,10 +3654,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="48" spans="1:8">
-      <c r="A48" s="9">
-        <v>44988</v>
-      </c>
+    <row r="48" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B48" s="6">
         <v>64317</v>
       </c>
@@ -3825,10 +3677,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="49" spans="1:8">
-      <c r="A49" s="9">
-        <v>44988</v>
-      </c>
+    <row r="49" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B49" s="6">
         <v>64180</v>
       </c>
@@ -3851,10 +3700,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="50" spans="1:8">
-      <c r="A50" s="9">
-        <v>44988</v>
-      </c>
+    <row r="50" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B50" s="6">
         <v>64275</v>
       </c>
@@ -3877,10 +3723,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="51" spans="1:8">
-      <c r="A51" s="9">
-        <v>44988</v>
-      </c>
+    <row r="51" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B51" s="6">
         <v>64280</v>
       </c>
@@ -3903,10 +3746,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="52" spans="1:8">
-      <c r="A52" s="9">
-        <v>44988</v>
-      </c>
+    <row r="52" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B52" s="6">
         <v>64285</v>
       </c>
@@ -3929,10 +3769,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="53" spans="1:8">
-      <c r="A53" s="9">
-        <v>44988</v>
-      </c>
+    <row r="53" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B53" s="6">
         <v>64319</v>
       </c>
@@ -3955,10 +3792,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="54" spans="1:8">
-      <c r="A54" s="9">
-        <v>44988</v>
-      </c>
+    <row r="54" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B54" s="6">
         <v>64188</v>
       </c>
@@ -3981,10 +3815,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="55" spans="1:8">
-      <c r="A55" s="9">
-        <v>44988</v>
-      </c>
+    <row r="55" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B55" s="6">
         <v>64813</v>
       </c>
@@ -4007,10 +3838,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="56" spans="1:8">
-      <c r="A56" s="9">
-        <v>44988</v>
-      </c>
+    <row r="56" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B56" s="6">
         <v>65257</v>
       </c>
@@ -4033,10 +3861,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="57" spans="1:8">
-      <c r="A57" s="9">
-        <v>44988</v>
-      </c>
+    <row r="57" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B57" s="6">
         <v>65309</v>
       </c>
@@ -4059,10 +3884,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="58" spans="1:8">
-      <c r="A58" s="9">
-        <v>44988</v>
-      </c>
+    <row r="58" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B58" s="6">
         <v>65585</v>
       </c>
@@ -4085,10 +3907,7 @@
         <v>564</v>
       </c>
     </row>
-    <row r="59" spans="1:8">
-      <c r="A59" s="9">
-        <v>44988</v>
-      </c>
+    <row r="59" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B59" s="6">
         <v>65586</v>
       </c>
@@ -4111,10 +3930,7 @@
         <v>566</v>
       </c>
     </row>
-    <row r="60" spans="1:8">
-      <c r="A60" s="9">
-        <v>44988</v>
-      </c>
+    <row r="60" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B60" s="6">
         <v>65291</v>
       </c>
@@ -4137,10 +3953,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="61" spans="1:8">
-      <c r="A61" s="9">
-        <v>44988</v>
-      </c>
+    <row r="61" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B61" s="6">
         <v>65406</v>
       </c>
@@ -4163,10 +3976,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="62" spans="1:8">
-      <c r="A62" s="9">
-        <v>44988</v>
-      </c>
+    <row r="62" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B62" s="6">
         <v>65241</v>
       </c>
@@ -4189,10 +3999,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="63" spans="1:8">
-      <c r="A63" s="9">
-        <v>44988</v>
-      </c>
+    <row r="63" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B63" s="6">
         <v>65293</v>
       </c>
@@ -4215,10 +4022,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="64" spans="1:8">
-      <c r="A64" s="9">
-        <v>44988</v>
-      </c>
+    <row r="64" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B64" s="6">
         <v>65408</v>
       </c>
@@ -4241,10 +4045,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="65" spans="1:8">
-      <c r="A65" s="9">
-        <v>44988</v>
-      </c>
+    <row r="65" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B65" s="6">
         <v>65253</v>
       </c>
@@ -4267,10 +4068,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="66" spans="1:8">
-      <c r="A66" s="9">
-        <v>44988</v>
-      </c>
+    <row r="66" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B66" s="6">
         <v>64202</v>
       </c>
@@ -4291,10 +4089,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="67" spans="1:8">
-      <c r="A67" s="9">
-        <v>44988</v>
-      </c>
+    <row r="67" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B67" s="6">
         <v>64206</v>
       </c>
@@ -4315,10 +4110,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="68" spans="1:8">
-      <c r="A68" s="9">
-        <v>44988</v>
-      </c>
+    <row r="68" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B68" s="6">
         <v>64210</v>
       </c>
@@ -4341,10 +4133,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="69" spans="1:8">
-      <c r="A69" s="9">
-        <v>44988</v>
-      </c>
+    <row r="69" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B69" s="6">
         <v>64214</v>
       </c>
@@ -4367,10 +4156,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="70" spans="1:8">
-      <c r="A70" s="9">
-        <v>44988</v>
-      </c>
+    <row r="70" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B70" s="6">
         <v>64218</v>
       </c>
@@ -4393,10 +4179,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="71" spans="1:8">
-      <c r="A71" s="9">
-        <v>44988</v>
-      </c>
+    <row r="71" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B71" s="6">
         <v>64222</v>
       </c>
@@ -4419,10 +4202,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="72" spans="1:8">
-      <c r="A72" s="9">
-        <v>44988</v>
-      </c>
+    <row r="72" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B72" s="6">
         <v>64227</v>
       </c>
@@ -4443,10 +4223,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="73" spans="1:8">
-      <c r="A73" s="9">
-        <v>44988</v>
-      </c>
+    <row r="73" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B73" s="6">
         <v>64231</v>
       </c>
@@ -4467,10 +4244,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="74" spans="1:8">
-      <c r="A74" s="9">
-        <v>44988</v>
-      </c>
+    <row r="74" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B74" s="6">
         <v>64236</v>
       </c>
@@ -4493,10 +4267,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="75" spans="1:8">
-      <c r="A75" s="9">
-        <v>44988</v>
-      </c>
+    <row r="75" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B75" s="6">
         <v>64307</v>
       </c>
@@ -4519,10 +4290,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="76" spans="1:8">
-      <c r="A76" s="9">
-        <v>44988</v>
-      </c>
+    <row r="76" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B76" s="6">
         <v>64456</v>
       </c>
@@ -4545,10 +4313,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="77" spans="1:8">
-      <c r="A77" s="9">
-        <v>44988</v>
-      </c>
+    <row r="77" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B77" s="6">
         <v>64460</v>
       </c>
@@ -4571,10 +4336,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="78" spans="1:8">
-      <c r="A78" s="9">
-        <v>44988</v>
-      </c>
+    <row r="78" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B78" s="6">
         <v>65726</v>
       </c>
@@ -4597,10 +4359,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="79" spans="1:8">
-      <c r="A79" s="9">
-        <v>44988</v>
-      </c>
+    <row r="79" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B79" s="6">
         <v>64459</v>
       </c>
@@ -4623,10 +4382,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="80" spans="1:8">
-      <c r="A80" s="9">
-        <v>44988</v>
-      </c>
+    <row r="80" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B80" s="6">
         <v>64303</v>
       </c>
@@ -4649,10 +4405,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="81" spans="1:8">
-      <c r="A81" s="9">
-        <v>44988</v>
-      </c>
+    <row r="81" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B81" s="6">
         <v>64335</v>
       </c>
@@ -4675,10 +4428,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="82" spans="1:8">
-      <c r="A82" s="9">
-        <v>44988</v>
-      </c>
+    <row r="82" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B82" s="6">
         <v>64812</v>
       </c>
@@ -4701,10 +4451,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="83" spans="1:8">
-      <c r="A83" s="9">
-        <v>44988</v>
-      </c>
+    <row r="83" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B83" s="6">
         <v>64195</v>
       </c>
@@ -4727,10 +4474,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="84" spans="1:8">
-      <c r="A84" s="9">
-        <v>44988</v>
-      </c>
+    <row r="84" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B84" s="6">
         <v>64856</v>
       </c>
@@ -4753,10 +4497,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="85" spans="1:8">
-      <c r="A85" s="9">
-        <v>44988</v>
-      </c>
+    <row r="85" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B85" s="6">
         <v>65541</v>
       </c>
@@ -4779,10 +4520,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="86" spans="1:8">
-      <c r="A86" s="9">
-        <v>44988</v>
-      </c>
+    <row r="86" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B86" s="6">
         <v>65153</v>
       </c>
@@ -4805,10 +4543,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="87" spans="1:8">
-      <c r="A87" s="9">
-        <v>44988</v>
-      </c>
+    <row r="87" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B87" s="6">
         <v>64159</v>
       </c>
@@ -4831,10 +4566,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="88" spans="1:8">
-      <c r="A88" s="9">
-        <v>44988</v>
-      </c>
+    <row r="88" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B88" s="6">
         <v>64179</v>
       </c>
@@ -4857,10 +4589,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="89" spans="1:8">
-      <c r="A89" s="9">
-        <v>44988</v>
-      </c>
+    <row r="89" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B89" s="6">
         <v>64274</v>
       </c>
@@ -4883,10 +4612,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="90" spans="1:8">
-      <c r="A90" s="9">
-        <v>44988</v>
-      </c>
+    <row r="90" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B90" s="6">
         <v>64279</v>
       </c>
@@ -4909,10 +4635,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="91" spans="1:8">
-      <c r="A91" s="9">
-        <v>44988</v>
-      </c>
+    <row r="91" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B91" s="6">
         <v>64284</v>
       </c>
@@ -4935,10 +4658,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="92" spans="1:8">
-      <c r="A92" s="9">
-        <v>44988</v>
-      </c>
+    <row r="92" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B92" s="6">
         <v>64318</v>
       </c>
@@ -4961,10 +4681,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="93" spans="1:8">
-      <c r="A93" s="9">
-        <v>44988</v>
-      </c>
+    <row r="93" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B93" s="6">
         <v>64163</v>
       </c>
@@ -4987,10 +4704,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="94" spans="1:8">
-      <c r="A94" s="9">
-        <v>44988</v>
-      </c>
+    <row r="94" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B94" s="6">
         <v>64183</v>
       </c>
@@ -5013,10 +4727,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="95" spans="1:8">
-      <c r="A95" s="9">
-        <v>44988</v>
-      </c>
+    <row r="95" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B95" s="6">
         <v>64289</v>
       </c>
@@ -5039,10 +4750,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="96" spans="1:8">
-      <c r="A96" s="9">
-        <v>44988</v>
-      </c>
+    <row r="96" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B96" s="6">
         <v>64323</v>
       </c>
@@ -5065,10 +4773,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="97" spans="1:8">
-      <c r="A97" s="9">
-        <v>44988</v>
-      </c>
+    <row r="97" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B97" s="6">
         <v>64486</v>
       </c>
@@ -5091,10 +4796,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="98" spans="1:8">
-      <c r="A98" s="9">
-        <v>44988</v>
-      </c>
+    <row r="98" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B98" s="6">
         <v>64489</v>
       </c>
@@ -5117,10 +4819,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="99" spans="1:8">
-      <c r="A99" s="9">
-        <v>44988</v>
-      </c>
+    <row r="99" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B99" s="6">
         <v>64490</v>
       </c>
@@ -5143,10 +4842,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="100" spans="1:8">
-      <c r="A100" s="9">
-        <v>44988</v>
-      </c>
+    <row r="100" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B100" s="6">
         <v>65156</v>
       </c>
@@ -5169,10 +4865,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="101" spans="1:8">
-      <c r="A101" s="9">
-        <v>44988</v>
-      </c>
+    <row r="101" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B101" s="6">
         <v>64774</v>
       </c>
@@ -5195,10 +4888,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="102" spans="1:8">
-      <c r="A102" s="9">
-        <v>44988</v>
-      </c>
+    <row r="102" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B102" s="6">
         <v>64197</v>
       </c>
@@ -5221,10 +4911,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="103" spans="1:8">
-      <c r="A103" s="9">
-        <v>44988</v>
-      </c>
+    <row r="103" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B103" s="6">
         <v>64148</v>
       </c>
@@ -5247,10 +4934,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="104" spans="1:8">
-      <c r="A104" s="9">
-        <v>44988</v>
-      </c>
+    <row r="104" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B104" s="6">
         <v>64152</v>
       </c>
@@ -5273,10 +4957,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="105" spans="1:8">
-      <c r="A105" s="9">
-        <v>44988</v>
-      </c>
+    <row r="105" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B105" s="6">
         <v>64175</v>
       </c>
@@ -5299,10 +4980,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="106" spans="1:8">
-      <c r="A106" s="9">
-        <v>44988</v>
-      </c>
+    <row r="106" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B106" s="6">
         <v>64249</v>
       </c>
@@ -5325,10 +5003,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="107" spans="1:8">
-      <c r="A107" s="9">
-        <v>44988</v>
-      </c>
+    <row r="107" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B107" s="6">
         <v>64253</v>
       </c>
@@ -5351,10 +5026,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="108" spans="1:8">
-      <c r="A108" s="9">
-        <v>44988</v>
-      </c>
+    <row r="108" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B108" s="6">
         <v>64257</v>
       </c>
@@ -5377,10 +5049,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="109" spans="1:8">
-      <c r="A109" s="9">
-        <v>44988</v>
-      </c>
+    <row r="109" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B109" s="6">
         <v>64261</v>
       </c>
@@ -5403,10 +5072,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="110" spans="1:8">
-      <c r="A110" s="9">
-        <v>44988</v>
-      </c>
+    <row r="110" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B110" s="6">
         <v>64310</v>
       </c>
@@ -5429,10 +5095,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="111" spans="1:8">
-      <c r="A111" s="9">
-        <v>44988</v>
-      </c>
+    <row r="111" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B111" s="6">
         <v>64458</v>
       </c>
@@ -5455,10 +5118,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="112" spans="1:8">
-      <c r="A112" s="9">
-        <v>44988</v>
-      </c>
+    <row r="112" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B112" s="6">
         <v>64265</v>
       </c>
@@ -5481,10 +5141,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="113" spans="1:8">
-      <c r="A113" s="9">
-        <v>44988</v>
-      </c>
+    <row r="113" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B113" s="6">
         <v>64270</v>
       </c>
@@ -5507,10 +5164,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="114" spans="1:8">
-      <c r="A114" s="9">
-        <v>44988</v>
-      </c>
+    <row r="114" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B114" s="6">
         <v>64314</v>
       </c>
@@ -5533,10 +5187,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="115" spans="1:8">
-      <c r="A115" s="9">
-        <v>44988</v>
-      </c>
+    <row r="115" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B115" s="6">
         <v>65273</v>
       </c>
@@ -5559,10 +5210,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="116" spans="1:8">
-      <c r="A116" s="9">
-        <v>44988</v>
-      </c>
+    <row r="116" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B116" s="6">
         <v>64192</v>
       </c>
@@ -5585,10 +5233,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="117" spans="1:8">
-      <c r="A117" s="9">
-        <v>44988</v>
-      </c>
+    <row r="117" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B117" s="6">
         <v>64880</v>
       </c>
@@ -5611,10 +5256,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="118" spans="1:8">
-      <c r="A118" s="9">
-        <v>44988</v>
-      </c>
+    <row r="118" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B118" s="6">
         <v>64461</v>
       </c>
@@ -5637,10 +5279,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="119" spans="1:8">
-      <c r="A119" s="9">
-        <v>44988</v>
-      </c>
+    <row r="119" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B119" s="6">
         <v>65294</v>
       </c>
@@ -5663,10 +5302,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="120" spans="1:8">
-      <c r="A120" s="9">
-        <v>44988</v>
-      </c>
+    <row r="120" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B120" s="6">
         <v>65409</v>
       </c>
@@ -5689,10 +5325,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="121" spans="1:8">
-      <c r="A121" s="9">
-        <v>44988</v>
-      </c>
+    <row r="121" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B121" s="6">
         <v>65292</v>
       </c>
@@ -5715,10 +5348,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="122" spans="1:8">
-      <c r="A122" s="9">
-        <v>44988</v>
-      </c>
+    <row r="122" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B122" s="6">
         <v>65407</v>
       </c>
@@ -5741,10 +5371,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="123" spans="1:8">
-      <c r="A123" s="9">
-        <v>44988</v>
-      </c>
+    <row r="123" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B123" s="6">
         <v>64240</v>
       </c>
@@ -5767,10 +5394,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="124" spans="1:8">
-      <c r="A124" s="9">
-        <v>44988</v>
-      </c>
+    <row r="124" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B124" s="6">
         <v>64244</v>
       </c>
@@ -5793,10 +5417,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="125" spans="1:8">
-      <c r="A125" s="9">
-        <v>44988</v>
-      </c>
+    <row r="125" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B125" s="6">
         <v>64785</v>
       </c>
@@ -5819,10 +5440,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="126" spans="1:8">
-      <c r="A126" s="9">
-        <v>44988</v>
-      </c>
+    <row r="126" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B126" s="6">
         <v>64238</v>
       </c>
@@ -5845,10 +5463,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="127" spans="1:8">
-      <c r="A127" s="9">
-        <v>44988</v>
-      </c>
+    <row r="127" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B127" s="6">
         <v>64242</v>
       </c>
@@ -5871,10 +5486,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="128" spans="1:8">
-      <c r="A128" s="9">
-        <v>44988</v>
-      </c>
+    <row r="128" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B128" s="6">
         <v>64309</v>
       </c>
@@ -5897,10 +5509,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="129" spans="1:8">
-      <c r="A129" s="9">
-        <v>44988</v>
-      </c>
+    <row r="129" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B129" s="6">
         <v>64154</v>
       </c>
@@ -5923,10 +5532,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="130" spans="1:8">
-      <c r="A130" s="9">
-        <v>44988</v>
-      </c>
+    <row r="130" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B130" s="6">
         <v>64177</v>
       </c>
@@ -5949,10 +5555,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="131" spans="1:8">
-      <c r="A131" s="9">
-        <v>44988</v>
-      </c>
+    <row r="131" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B131" s="6">
         <v>64269</v>
       </c>
@@ -5975,10 +5578,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="132" spans="1:8">
-      <c r="A132" s="9">
-        <v>44988</v>
-      </c>
+    <row r="132" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B132" s="6">
         <v>64273</v>
       </c>
@@ -6001,10 +5601,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="133" spans="1:8">
-      <c r="A133" s="9">
-        <v>44988</v>
-      </c>
+    <row r="133" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B133" s="6">
         <v>64315</v>
       </c>
@@ -6027,10 +5624,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="134" spans="1:8">
-      <c r="A134" s="9">
-        <v>44988</v>
-      </c>
+    <row r="134" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B134" s="6">
         <v>64136</v>
       </c>
@@ -6051,10 +5645,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="135" spans="1:8">
-      <c r="A135" s="9">
-        <v>44988</v>
-      </c>
+    <row r="135" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B135" s="6">
         <v>64140</v>
       </c>
@@ -6077,10 +5668,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="136" spans="1:8">
-      <c r="A136" s="9">
-        <v>44988</v>
-      </c>
+    <row r="136" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B136" s="6">
         <v>64170</v>
       </c>
@@ -6103,10 +5691,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="137" spans="1:8">
-      <c r="A137" s="9">
-        <v>44988</v>
-      </c>
+    <row r="137" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B137" s="6">
         <v>65546</v>
       </c>
@@ -6129,10 +5714,7 @@
         <v>561</v>
       </c>
     </row>
-    <row r="138" spans="1:8">
-      <c r="A138" s="9">
-        <v>44988</v>
-      </c>
+    <row r="138" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B138" s="6">
         <v>65547</v>
       </c>
@@ -6155,10 +5737,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="139" spans="1:8">
-      <c r="A139" s="9">
-        <v>44988</v>
-      </c>
+    <row r="139" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B139" s="6">
         <v>64144</v>
       </c>
@@ -6181,10 +5760,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="140" spans="1:8">
-      <c r="A140" s="9">
-        <v>44988</v>
-      </c>
+    <row r="140" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B140" s="6">
         <v>64147</v>
       </c>
@@ -6207,10 +5783,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="141" spans="1:8">
-      <c r="A141" s="9">
-        <v>44988</v>
-      </c>
+    <row r="141" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B141" s="6">
         <v>64174</v>
       </c>
@@ -6233,10 +5806,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="142" spans="1:8">
-      <c r="A142" s="9">
-        <v>44988</v>
-      </c>
+    <row r="142" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B142" s="6">
         <v>65254</v>
       </c>
@@ -6259,10 +5829,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="143" spans="1:8">
-      <c r="A143" s="9">
-        <v>44988</v>
-      </c>
+    <row r="143" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B143" s="6">
         <v>64814</v>
       </c>
@@ -6285,10 +5852,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="144" spans="1:8">
-      <c r="A144" s="9">
-        <v>44988</v>
-      </c>
+    <row r="144" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B144" s="6">
         <v>64815</v>
       </c>
@@ -6311,10 +5875,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="145" spans="1:8">
-      <c r="A145" s="9">
-        <v>44988</v>
-      </c>
+    <row r="145" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B145" s="6">
         <v>64196</v>
       </c>
@@ -6337,10 +5898,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="146" spans="1:8">
-      <c r="A146" s="9">
-        <v>44988</v>
-      </c>
+    <row r="146" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B146" s="6">
         <v>64291</v>
       </c>
@@ -6363,10 +5921,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="147" spans="1:8">
-      <c r="A147" s="9">
-        <v>44988</v>
-      </c>
+    <row r="147" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B147" s="6">
         <v>64162</v>
       </c>
@@ -6389,10 +5944,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="148" spans="1:8">
-      <c r="A148" s="9">
-        <v>44988</v>
-      </c>
+    <row r="148" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B148" s="6">
         <v>64182</v>
       </c>
@@ -6415,10 +5967,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="149" spans="1:8">
-      <c r="A149" s="9">
-        <v>44988</v>
-      </c>
+    <row r="149" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B149" s="6">
         <v>65157</v>
       </c>
@@ -6441,10 +5990,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="150" spans="1:8">
-      <c r="A150" s="9">
-        <v>44988</v>
-      </c>
+    <row r="150" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B150" s="6">
         <v>64191</v>
       </c>
@@ -6467,10 +6013,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="151" spans="1:8">
-      <c r="A151" s="9">
-        <v>44988</v>
-      </c>
+    <row r="151" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B151" s="6">
         <v>64290</v>
       </c>
@@ -6493,10 +6036,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="152" spans="1:8">
-      <c r="A152" s="9">
-        <v>44988</v>
-      </c>
+    <row r="152" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B152" s="6">
         <v>64325</v>
       </c>
@@ -6519,10 +6059,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="153" spans="1:8">
-      <c r="A153" s="9">
-        <v>44988</v>
-      </c>
+    <row r="153" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B153" s="6">
         <v>64300</v>
       </c>
@@ -6545,10 +6082,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="154" spans="1:8">
-      <c r="A154" s="9">
-        <v>44988</v>
-      </c>
+    <row r="154" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B154" s="6">
         <v>64329</v>
       </c>
@@ -6571,10 +6105,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="155" spans="1:8">
-      <c r="A155" s="9">
-        <v>44988</v>
-      </c>
+    <row r="155" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B155" s="6">
         <v>64333</v>
       </c>
@@ -6597,10 +6128,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="156" spans="1:8">
-      <c r="A156" s="9">
-        <v>44988</v>
-      </c>
+    <row r="156" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B156" s="6">
         <v>65278</v>
       </c>
@@ -6623,10 +6151,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="157" spans="1:8">
-      <c r="A157" s="9">
-        <v>44988</v>
-      </c>
+    <row r="157" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B157" s="6">
         <v>64457</v>
       </c>
@@ -6649,10 +6174,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="158" spans="1:8">
-      <c r="A158" s="9">
-        <v>44988</v>
-      </c>
+    <row r="158" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B158" s="6">
         <v>64487</v>
       </c>
@@ -6675,10 +6197,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="159" spans="1:8">
-      <c r="A159" s="9">
-        <v>44988</v>
-      </c>
+    <row r="159" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B159" s="6">
         <v>64475</v>
       </c>
@@ -6701,10 +6220,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="160" spans="1:8">
-      <c r="A160" s="9">
-        <v>44988</v>
-      </c>
+    <row r="160" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B160" s="6">
         <v>64302</v>
       </c>
@@ -6727,10 +6243,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="161" spans="1:8">
-      <c r="A161" s="9">
-        <v>44988</v>
-      </c>
+    <row r="161" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B161" s="6">
         <v>64330</v>
       </c>
@@ -6753,10 +6266,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="162" spans="1:8">
-      <c r="A162" s="9">
-        <v>44988</v>
-      </c>
+    <row r="162" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B162" s="6">
         <v>64334</v>
       </c>
@@ -6779,10 +6289,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="163" spans="1:8">
-      <c r="A163" s="9">
-        <v>44988</v>
-      </c>
+    <row r="163" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B163" s="6">
         <v>64339</v>
       </c>
@@ -6805,10 +6312,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="164" spans="1:8">
-      <c r="A164" s="9">
-        <v>44988</v>
-      </c>
+    <row r="164" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B164" s="6">
         <v>64799</v>
       </c>
@@ -6831,10 +6335,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="165" spans="1:8">
-      <c r="A165" s="9">
-        <v>44988</v>
-      </c>
+    <row r="165" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B165" s="6">
         <v>65311</v>
       </c>
@@ -6857,10 +6358,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="166" spans="1:8">
-      <c r="A166" s="9">
-        <v>44988</v>
-      </c>
+    <row r="166" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B166" s="6">
         <v>65587</v>
       </c>
@@ -6883,10 +6381,7 @@
         <v>564</v>
       </c>
     </row>
-    <row r="167" spans="1:8">
-      <c r="A167" s="9">
-        <v>44988</v>
-      </c>
+    <row r="167" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B167" s="6">
         <v>65588</v>
       </c>
@@ -6909,10 +6404,7 @@
         <v>566</v>
       </c>
     </row>
-    <row r="168" spans="1:8">
-      <c r="A168" s="9">
-        <v>44988</v>
-      </c>
+    <row r="168" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B168" s="6">
         <v>65317</v>
       </c>
@@ -6935,10 +6427,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="169" spans="1:8">
-      <c r="A169" s="9">
-        <v>44988</v>
-      </c>
+    <row r="169" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B169" s="6">
         <v>65318</v>
       </c>
@@ -6961,10 +6450,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="170" spans="1:8">
-      <c r="A170" s="9">
-        <v>44988</v>
-      </c>
+    <row r="170" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B170" s="6">
         <v>65319</v>
       </c>
@@ -6987,10 +6473,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="171" spans="1:8">
-      <c r="A171" s="9">
-        <v>44988</v>
-      </c>
+    <row r="171" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B171" s="6">
         <v>65320</v>
       </c>
@@ -7013,10 +6496,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="172" spans="1:8">
-      <c r="A172" s="9">
-        <v>44988</v>
-      </c>
+    <row r="172" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B172" s="6">
         <v>65321</v>
       </c>
@@ -7039,10 +6519,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="173" spans="1:8">
-      <c r="A173" s="9">
-        <v>44988</v>
-      </c>
+    <row r="173" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B173" s="6">
         <v>65258</v>
       </c>
@@ -7065,10 +6542,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="174" spans="1:8">
-      <c r="A174" s="9">
-        <v>44988</v>
-      </c>
+    <row r="174" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B174" s="6">
         <v>65279</v>
       </c>
@@ -7091,10 +6565,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="175" spans="1:8">
-      <c r="A175" s="9">
-        <v>44988</v>
-      </c>
+    <row r="175" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B175" s="6">
         <v>65280</v>
       </c>
@@ -7117,10 +6588,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="176" spans="1:8">
-      <c r="A176" s="9">
-        <v>44988</v>
-      </c>
+    <row r="176" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B176" s="6">
         <v>65281</v>
       </c>
@@ -7143,10 +6611,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="177" spans="1:8">
-      <c r="A177" s="9">
-        <v>44988</v>
-      </c>
+    <row r="177" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B177" s="6">
         <v>65282</v>
       </c>
@@ -7169,10 +6634,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="178" spans="1:8">
-      <c r="A178" s="9">
-        <v>44988</v>
-      </c>
+    <row r="178" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B178" s="6">
         <v>65295</v>
       </c>
@@ -7195,10 +6657,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="179" spans="1:8">
-      <c r="A179" s="9">
-        <v>44988</v>
-      </c>
+    <row r="179" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B179" s="6">
         <v>65296</v>
       </c>
@@ -7221,10 +6680,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="180" spans="1:8">
-      <c r="A180" s="9">
-        <v>44988</v>
-      </c>
+    <row r="180" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B180" s="6">
         <v>65297</v>
       </c>
@@ -7247,10 +6703,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="181" spans="1:8">
-      <c r="A181" s="9">
-        <v>44988</v>
-      </c>
+    <row r="181" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B181" s="6">
         <v>65298</v>
       </c>
@@ -7273,10 +6726,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="182" spans="1:8">
-      <c r="A182" s="9">
-        <v>44988</v>
-      </c>
+    <row r="182" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B182" s="6">
         <v>64338</v>
       </c>
@@ -7299,10 +6749,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="183" spans="1:8">
-      <c r="A183" s="9">
-        <v>44988</v>
-      </c>
+    <row r="183" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B183" s="6">
         <v>64250</v>
       </c>
@@ -7325,10 +6772,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="184" spans="1:8">
-      <c r="A184" s="9">
-        <v>44988</v>
-      </c>
+    <row r="184" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B184" s="6">
         <v>64254</v>
       </c>
@@ -7351,10 +6795,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="185" spans="1:8">
-      <c r="A185" s="9">
-        <v>44988</v>
-      </c>
+    <row r="185" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B185" s="6">
         <v>64258</v>
       </c>
@@ -7377,10 +6818,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="186" spans="1:8">
-      <c r="A186" s="9">
-        <v>44988</v>
-      </c>
+    <row r="186" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B186" s="6">
         <v>64262</v>
       </c>
@@ -7403,10 +6841,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="187" spans="1:8">
-      <c r="A187" s="9">
-        <v>44988</v>
-      </c>
+    <row r="187" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B187" s="6">
         <v>64311</v>
       </c>
@@ -7429,10 +6864,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="188" spans="1:8">
-      <c r="A188" s="9">
-        <v>44988</v>
-      </c>
+    <row r="188" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B188" s="6">
         <v>64143</v>
       </c>
@@ -7455,10 +6887,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="189" spans="1:8">
-      <c r="A189" s="9">
-        <v>44988</v>
-      </c>
+    <row r="189" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B189" s="6">
         <v>64146</v>
       </c>
@@ -7481,10 +6910,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="190" spans="1:8">
-      <c r="A190" s="9">
-        <v>44988</v>
-      </c>
+    <row r="190" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B190" s="6">
         <v>64173</v>
       </c>
@@ -7507,10 +6933,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="191" spans="1:8">
-      <c r="A191" s="9">
-        <v>44988</v>
-      </c>
+    <row r="191" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B191" s="6">
         <v>64190</v>
       </c>
@@ -7533,10 +6956,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="192" spans="1:8">
-      <c r="A192" s="9">
-        <v>44988</v>
-      </c>
+    <row r="192" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B192" s="6">
         <v>64326</v>
       </c>
@@ -7559,10 +6979,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="193" spans="1:8">
-      <c r="A193" s="9">
-        <v>44988</v>
-      </c>
+    <row r="193" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B193" s="6">
         <v>64757</v>
       </c>
@@ -7585,10 +7002,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="194" spans="1:8">
-      <c r="A194" s="9">
-        <v>44988</v>
-      </c>
+    <row r="194" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B194" s="6">
         <v>64808</v>
       </c>
@@ -7609,10 +7023,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="195" spans="1:8">
-      <c r="A195" s="9">
-        <v>44988</v>
-      </c>
+    <row r="195" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B195" s="6">
         <v>64488</v>
       </c>
@@ -7635,10 +7046,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="196" spans="1:8">
-      <c r="A196" s="9">
-        <v>44988</v>
-      </c>
+    <row r="196" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B196" s="6">
         <v>64151</v>
       </c>
@@ -7661,10 +7069,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="197" spans="1:8">
-      <c r="A197" s="9">
-        <v>44988</v>
-      </c>
+    <row r="197" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B197" s="6">
         <v>64155</v>
       </c>
@@ -7687,10 +7092,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="198" spans="1:8">
-      <c r="A198" s="9">
-        <v>44988</v>
-      </c>
+    <row r="198" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B198" s="6">
         <v>64178</v>
       </c>
@@ -7713,10 +7115,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="199" spans="1:8">
-      <c r="A199" s="9">
-        <v>44988</v>
-      </c>
+    <row r="199" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B199" s="6">
         <v>65314</v>
       </c>
@@ -7739,10 +7138,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="200" spans="1:8">
-      <c r="A200" s="9">
-        <v>44988</v>
-      </c>
+    <row r="200" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B200" s="6">
         <v>65548</v>
       </c>
@@ -7763,10 +7159,7 @@
         <v>564</v>
       </c>
     </row>
-    <row r="201" spans="1:8">
-      <c r="A201" s="9">
-        <v>44988</v>
-      </c>
+    <row r="201" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B201" s="6">
         <v>65549</v>
       </c>
@@ -7789,10 +7182,7 @@
         <v>566</v>
       </c>
     </row>
-    <row r="202" spans="1:8">
-      <c r="A202" s="9">
-        <v>44988</v>
-      </c>
+    <row r="202" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B202" s="6">
         <v>64239</v>
       </c>
@@ -7815,10 +7205,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="203" spans="1:8">
-      <c r="A203" s="9">
-        <v>44988</v>
-      </c>
+    <row r="203" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B203" s="6">
         <v>64243</v>
       </c>
@@ -7841,10 +7228,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="204" spans="1:8">
-      <c r="A204" s="9">
-        <v>44988</v>
-      </c>
+    <row r="204" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B204" s="6">
         <v>65159</v>
       </c>
@@ -7867,10 +7251,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="205" spans="1:8">
-      <c r="A205" s="9">
-        <v>44988</v>
-      </c>
+    <row r="205" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B205" s="6">
         <v>64164</v>
       </c>
@@ -7893,10 +7274,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="206" spans="1:8">
-      <c r="A206" s="9">
-        <v>44988</v>
-      </c>
+    <row r="206" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B206" s="6">
         <v>64184</v>
       </c>
@@ -7919,10 +7297,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="207" spans="1:8">
-      <c r="A207" s="9">
-        <v>44988</v>
-      </c>
+    <row r="207" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B207" s="6">
         <v>65276</v>
       </c>
@@ -7945,10 +7320,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="208" spans="1:8">
-      <c r="A208" s="9">
-        <v>44988</v>
-      </c>
+    <row r="208" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B208" s="6">
         <v>65403</v>
       </c>
@@ -7971,10 +7343,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="209" spans="1:8">
-      <c r="A209" s="9">
-        <v>44988</v>
-      </c>
+    <row r="209" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B209" s="6">
         <v>64816</v>
       </c>
@@ -7997,10 +7366,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="210" spans="1:8">
-      <c r="A210" s="9">
-        <v>44988</v>
-      </c>
+    <row r="210" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B210" s="6">
         <v>64800</v>
       </c>
@@ -8023,10 +7389,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="211" spans="1:8">
-      <c r="A211" s="9">
-        <v>44988</v>
-      </c>
+    <row r="211" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B211" s="6">
         <v>64476</v>
       </c>
@@ -8049,10 +7412,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="212" spans="1:8">
-      <c r="A212" s="9">
-        <v>44988</v>
-      </c>
+    <row r="212" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B212" s="6">
         <v>64474</v>
       </c>
@@ -8075,10 +7435,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="213" spans="1:8">
-      <c r="A213" s="9">
-        <v>44988</v>
-      </c>
+    <row r="213" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B213" s="6">
         <v>64267</v>
       </c>
@@ -8101,10 +7458,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="214" spans="1:8">
-      <c r="A214" s="9">
-        <v>44988</v>
-      </c>
+    <row r="214" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B214" s="6">
         <v>64161</v>
       </c>
@@ -8127,10 +7481,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="215" spans="1:8">
-      <c r="A215" s="9">
-        <v>44988</v>
-      </c>
+    <row r="215" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B215" s="6">
         <v>64181</v>
       </c>
@@ -8153,10 +7504,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="216" spans="1:8">
-      <c r="A216" s="9">
-        <v>44988</v>
-      </c>
+    <row r="216" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B216" s="6">
         <v>64251</v>
       </c>
@@ -8179,10 +7527,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="217" spans="1:8">
-      <c r="A217" s="9">
-        <v>44988</v>
-      </c>
+    <row r="217" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B217" s="6">
         <v>64255</v>
       </c>
@@ -8205,10 +7550,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="218" spans="1:8">
-      <c r="A218" s="9">
-        <v>44988</v>
-      </c>
+    <row r="218" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B218" s="6">
         <v>64259</v>
       </c>
@@ -8231,10 +7573,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="219" spans="1:8">
-      <c r="A219" s="9">
-        <v>44988</v>
-      </c>
+    <row r="219" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B219" s="6">
         <v>64263</v>
       </c>
@@ -8257,10 +7596,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="220" spans="1:8">
-      <c r="A220" s="9">
-        <v>44988</v>
-      </c>
+    <row r="220" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B220" s="6">
         <v>64312</v>
       </c>
@@ -8283,10 +7619,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="221" spans="1:8">
-      <c r="A221" s="9">
-        <v>44988</v>
-      </c>
+    <row r="221" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B221" s="6">
         <v>65290</v>
       </c>
@@ -8309,10 +7642,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="222" spans="1:8">
-      <c r="A222" s="9">
-        <v>44988</v>
-      </c>
+    <row r="222" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B222" s="6">
         <v>65405</v>
       </c>
@@ -8335,10 +7665,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="223" spans="1:8">
-      <c r="A223" s="9">
-        <v>44988</v>
-      </c>
+    <row r="223" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B223" s="6">
         <v>65277</v>
       </c>
@@ -8361,10 +7688,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="224" spans="1:8">
-      <c r="A224" s="9">
-        <v>44988</v>
-      </c>
+    <row r="224" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B224" s="6">
         <v>65404</v>
       </c>
@@ -8387,10 +7711,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="225" spans="1:8">
-      <c r="A225" s="9">
-        <v>44988</v>
-      </c>
+    <row r="225" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B225" s="6">
         <v>64134</v>
       </c>
@@ -8413,10 +7734,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="226" spans="1:8">
-      <c r="A226" s="9">
-        <v>44988</v>
-      </c>
+    <row r="226" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B226" s="6">
         <v>64138</v>
       </c>
@@ -8439,10 +7757,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="227" spans="1:8">
-      <c r="A227" s="9">
-        <v>44988</v>
-      </c>
+    <row r="227" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B227" s="6">
         <v>64168</v>
       </c>
@@ -8465,10 +7780,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="228" spans="1:8">
-      <c r="A228" s="9">
-        <v>44988</v>
-      </c>
+    <row r="228" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B228" s="6">
         <v>64199</v>
       </c>
@@ -8491,10 +7803,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="229" spans="1:8">
-      <c r="A229" s="9">
-        <v>44988</v>
-      </c>
+    <row r="229" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B229" s="6">
         <v>64203</v>
       </c>
@@ -8517,10 +7826,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="230" spans="1:8">
-      <c r="A230" s="9">
-        <v>44988</v>
-      </c>
+    <row r="230" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B230" s="6">
         <v>64207</v>
       </c>
@@ -8543,10 +7849,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="231" spans="1:8">
-      <c r="A231" s="9">
-        <v>44988</v>
-      </c>
+    <row r="231" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B231" s="6">
         <v>64211</v>
       </c>
@@ -8569,10 +7872,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="232" spans="1:8">
-      <c r="A232" s="9">
-        <v>44988</v>
-      </c>
+    <row r="232" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B232" s="6">
         <v>64215</v>
       </c>
@@ -8595,10 +7895,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="233" spans="1:8">
-      <c r="A233" s="9">
-        <v>44988</v>
-      </c>
+    <row r="233" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B233" s="6">
         <v>64219</v>
       </c>
@@ -8621,10 +7918,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="234" spans="1:8">
-      <c r="A234" s="9">
-        <v>44988</v>
-      </c>
+    <row r="234" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B234" s="6">
         <v>64223</v>
       </c>
@@ -8647,10 +7941,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="235" spans="1:8">
-      <c r="A235" s="9">
-        <v>44988</v>
-      </c>
+    <row r="235" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B235" s="6">
         <v>64228</v>
       </c>
@@ -8673,10 +7964,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="236" spans="1:8">
-      <c r="A236" s="9">
-        <v>44988</v>
-      </c>
+    <row r="236" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B236" s="6">
         <v>64233</v>
       </c>
@@ -8699,10 +7987,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="237" spans="1:8">
-      <c r="A237" s="9">
-        <v>44988</v>
-      </c>
+    <row r="237" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B237" s="6">
         <v>64304</v>
       </c>
@@ -8725,10 +8010,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="238" spans="1:8">
-      <c r="A238" s="9">
-        <v>44988</v>
-      </c>
+    <row r="238" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B238" s="6">
         <v>65504</v>
       </c>
@@ -8749,10 +8031,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="239" spans="1:8">
-      <c r="A239" s="9">
-        <v>44988</v>
-      </c>
+    <row r="239" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B239" s="6">
         <v>65508</v>
       </c>
@@ -8775,10 +8054,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="240" spans="1:8">
-      <c r="A240" s="9">
-        <v>44988</v>
-      </c>
+    <row r="240" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B240" s="6">
         <v>64142</v>
       </c>
@@ -8801,10 +8077,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="241" spans="1:8">
-      <c r="A241" s="9">
-        <v>44988</v>
-      </c>
+    <row r="241" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B241" s="6">
         <v>64145</v>
       </c>
@@ -8827,10 +8100,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="242" spans="1:8">
-      <c r="A242" s="9">
-        <v>44988</v>
-      </c>
+    <row r="242" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B242" s="6">
         <v>64172</v>
       </c>
@@ -8853,10 +8123,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="243" spans="1:8">
-      <c r="A243" s="9">
-        <v>44988</v>
-      </c>
+    <row r="243" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B243" s="6">
         <v>64237</v>
       </c>
@@ -8879,10 +8146,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="244" spans="1:8">
-      <c r="A244" s="9">
-        <v>44988</v>
-      </c>
+    <row r="244" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B244" s="6">
         <v>64241</v>
       </c>
@@ -8905,10 +8169,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="245" spans="1:8">
-      <c r="A245" s="9">
-        <v>44988</v>
-      </c>
+    <row r="245" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B245" s="6">
         <v>64189</v>
       </c>
@@ -8931,10 +8192,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="246" spans="1:8">
-      <c r="A246" s="9">
-        <v>44988</v>
-      </c>
+    <row r="246" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B246" s="6">
         <v>64324</v>
       </c>
@@ -8957,10 +8215,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="247" spans="1:8">
-      <c r="A247" s="9">
-        <v>44988</v>
-      </c>
+    <row r="247" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B247" s="6">
         <v>65161</v>
       </c>
@@ -8983,10 +8238,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="248" spans="1:8">
-      <c r="A248" s="9">
-        <v>44988</v>
-      </c>
+    <row r="248" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B248" s="6">
         <v>65256</v>
       </c>
@@ -9009,10 +8261,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="249" spans="1:8">
-      <c r="A249" s="9">
-        <v>44988</v>
-      </c>
+    <row r="249" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B249" s="6">
         <v>65542</v>
       </c>
@@ -9035,10 +8284,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="250" spans="1:8">
-      <c r="A250" s="9">
-        <v>44988</v>
-      </c>
+    <row r="250" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B250" s="6">
         <v>65316</v>
       </c>
@@ -9061,10 +8307,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="251" spans="1:8">
-      <c r="A251" s="9">
-        <v>44988</v>
-      </c>
+    <row r="251" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B251" s="6">
         <v>65583</v>
       </c>
@@ -9087,10 +8330,7 @@
         <v>564</v>
       </c>
     </row>
-    <row r="252" spans="1:8">
-      <c r="A252" s="9">
-        <v>44988</v>
-      </c>
+    <row r="252" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B252" s="6">
         <v>65584</v>
       </c>
@@ -9113,10 +8353,7 @@
         <v>566</v>
       </c>
     </row>
-    <row r="253" spans="1:8">
-      <c r="A253" s="9">
-        <v>44988</v>
-      </c>
+    <row r="253" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B253" s="6">
         <v>64165</v>
       </c>
@@ -9139,10 +8376,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="254" spans="1:8">
-      <c r="A254" s="9">
-        <v>44988</v>
-      </c>
+    <row r="254" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B254" s="6">
         <v>64185</v>
       </c>
@@ -9165,10 +8399,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="255" spans="1:8">
-      <c r="A255" s="9">
-        <v>44988</v>
-      </c>
+    <row r="255" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B255" s="6">
         <v>64276</v>
       </c>
@@ -9191,10 +8422,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="256" spans="1:8">
-      <c r="A256" s="9">
-        <v>44988</v>
-      </c>
+    <row r="256" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B256" s="6">
         <v>64281</v>
       </c>
@@ -9217,10 +8445,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="257" spans="1:8">
-      <c r="A257" s="9">
-        <v>44988</v>
-      </c>
+    <row r="257" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B257" s="6">
         <v>64286</v>
       </c>
@@ -9243,10 +8468,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="258" spans="1:8">
-      <c r="A258" s="9">
-        <v>44988</v>
-      </c>
+    <row r="258" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B258" s="6">
         <v>64320</v>
       </c>
@@ -9269,10 +8491,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="259" spans="1:8">
-      <c r="A259" s="9">
-        <v>44988</v>
-      </c>
+    <row r="259" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B259" s="6">
         <v>64477</v>
       </c>
@@ -9295,10 +8514,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="260" spans="1:8">
-      <c r="A260" s="9">
-        <v>44988</v>
-      </c>
+    <row r="260" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B260" s="6">
         <v>65543</v>
       </c>
@@ -9319,10 +8535,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="261" spans="1:8">
-      <c r="A261" s="9">
-        <v>44988</v>
-      </c>
+    <row r="261" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B261" s="6">
         <v>64473</v>
       </c>
@@ -9345,10 +8558,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="262" spans="1:8">
-      <c r="A262" s="9">
-        <v>44988</v>
-      </c>
+    <row r="262" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B262" s="6">
         <v>64472</v>
       </c>
@@ -9371,10 +8581,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="263" spans="1:8">
-      <c r="A263" s="9">
-        <v>44988</v>
-      </c>
+    <row r="263" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B263" s="6">
         <v>64167</v>
       </c>
@@ -9397,10 +8604,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="264" spans="1:8">
-      <c r="A264" s="9">
-        <v>44988</v>
-      </c>
+    <row r="264" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B264" s="6">
         <v>64198</v>
       </c>
@@ -9423,10 +8627,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="265" spans="1:8">
-      <c r="A265" s="9">
-        <v>44988</v>
-      </c>
+    <row r="265" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B265" s="6">
         <v>64266</v>
       </c>
@@ -9449,10 +8650,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="266" spans="1:8">
-      <c r="A266" s="9">
-        <v>44988</v>
-      </c>
+    <row r="266" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B266" s="6">
         <v>64271</v>
       </c>
@@ -9475,10 +8673,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="267" spans="1:8">
-      <c r="A267" s="9">
-        <v>44988</v>
-      </c>
+    <row r="267" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B267" s="6">
         <v>64316</v>
       </c>
@@ -9501,10 +8696,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="268" spans="1:8">
-      <c r="A268" s="9">
-        <v>44988</v>
-      </c>
+    <row r="268" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B268" s="6">
         <v>64491</v>
       </c>
@@ -9527,10 +8719,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="269" spans="1:8">
-      <c r="A269" s="9">
-        <v>44988</v>
-      </c>
+    <row r="269" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B269" s="6">
         <v>64809</v>
       </c>
@@ -9553,10 +8742,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="270" spans="1:8">
-      <c r="A270" s="9">
-        <v>44988</v>
-      </c>
+    <row r="270" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B270" s="6">
         <v>64807</v>
       </c>
@@ -9579,10 +8765,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="271" spans="1:8">
-      <c r="A271" s="9">
-        <v>44988</v>
-      </c>
+    <row r="271" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B271" s="6">
         <v>64492</v>
       </c>
@@ -9605,10 +8788,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="272" spans="1:8">
-      <c r="A272" s="9">
-        <v>44988</v>
-      </c>
+    <row r="272" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B272" s="6">
         <v>64135</v>
       </c>
@@ -9631,10 +8811,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="273" spans="1:8">
-      <c r="A273" s="9">
-        <v>44988</v>
-      </c>
+    <row r="273" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B273" s="6">
         <v>64139</v>
       </c>
@@ -9657,10 +8834,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="274" spans="1:8">
-      <c r="A274" s="9">
-        <v>44988</v>
-      </c>
+    <row r="274" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B274" s="6">
         <v>64169</v>
       </c>
@@ -9683,10 +8857,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="275" spans="1:8">
-      <c r="A275" s="9">
-        <v>44988</v>
-      </c>
+    <row r="275" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B275" s="6">
         <v>64200</v>
       </c>
@@ -9709,10 +8880,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="276" spans="1:8">
-      <c r="A276" s="9">
-        <v>44988</v>
-      </c>
+    <row r="276" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B276" s="6">
         <v>64204</v>
       </c>
@@ -9735,10 +8903,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="277" spans="1:8">
-      <c r="A277" s="9">
-        <v>44988</v>
-      </c>
+    <row r="277" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B277" s="6">
         <v>64208</v>
       </c>
@@ -9761,10 +8926,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="278" spans="1:8">
-      <c r="A278" s="9">
-        <v>44988</v>
-      </c>
+    <row r="278" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B278" s="6">
         <v>64212</v>
       </c>
@@ -9787,10 +8949,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="279" spans="1:8">
-      <c r="A279" s="9">
-        <v>44988</v>
-      </c>
+    <row r="279" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B279" s="6">
         <v>64216</v>
       </c>
@@ -9813,10 +8972,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="280" spans="1:8">
-      <c r="A280" s="9">
-        <v>44988</v>
-      </c>
+    <row r="280" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B280" s="6">
         <v>64220</v>
       </c>
@@ -9839,10 +8995,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="281" spans="1:8">
-      <c r="A281" s="9">
-        <v>44988</v>
-      </c>
+    <row r="281" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B281" s="6">
         <v>64225</v>
       </c>
@@ -9865,10 +9018,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="282" spans="1:8">
-      <c r="A282" s="9">
-        <v>44988</v>
-      </c>
+    <row r="282" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B282" s="6">
         <v>64229</v>
       </c>
@@ -9891,10 +9041,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="283" spans="1:8">
-      <c r="A283" s="9">
-        <v>44988</v>
-      </c>
+    <row r="283" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B283" s="6">
         <v>64234</v>
       </c>
@@ -9917,10 +9064,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="284" spans="1:8">
-      <c r="A284" s="9">
-        <v>44988</v>
-      </c>
+    <row r="284" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B284" s="6">
         <v>64305</v>
       </c>
@@ -9943,10 +9087,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="285" spans="1:8">
-      <c r="A285" s="9">
-        <v>44988</v>
-      </c>
+    <row r="285" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B285" s="6">
         <v>65550</v>
       </c>
@@ -9969,10 +9110,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="286" spans="1:8">
-      <c r="A286" s="9">
-        <v>44988</v>
-      </c>
+    <row r="286" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B286" s="6">
         <v>65551</v>
       </c>
@@ -9995,10 +9133,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="287" spans="1:8">
-      <c r="A287" s="9">
-        <v>44988</v>
-      </c>
+    <row r="287" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B287" s="6">
         <v>64327</v>
       </c>
@@ -10021,10 +9156,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="288" spans="1:8">
-      <c r="A288" s="9">
-        <v>44988</v>
-      </c>
+    <row r="288" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B288" s="6">
         <v>64810</v>
       </c>
@@ -10047,10 +9179,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="289" spans="1:8">
-      <c r="A289" s="9">
-        <v>44988</v>
-      </c>
+    <row r="289" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B289" s="6">
         <v>65244</v>
       </c>
@@ -10073,10 +9202,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="290" spans="1:8">
-      <c r="A290" s="9">
-        <v>44988</v>
-      </c>
+    <row r="290" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B290" s="6">
         <v>65162</v>
       </c>
@@ -10099,10 +9225,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="291" spans="1:8">
-      <c r="A291" s="9">
-        <v>44988</v>
-      </c>
+    <row r="291" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B291" s="6">
         <v>64278</v>
       </c>
@@ -10125,10 +9248,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="292" spans="1:8">
-      <c r="A292" s="9">
-        <v>44988</v>
-      </c>
+    <row r="292" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B292" s="6">
         <v>64283</v>
       </c>
@@ -10151,10 +9271,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="293" spans="1:8">
-      <c r="A293" s="9">
-        <v>44988</v>
-      </c>
+    <row r="293" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B293" s="6">
         <v>64288</v>
       </c>
@@ -10177,10 +9294,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="294" spans="1:8">
-      <c r="A294" s="9">
-        <v>44988</v>
-      </c>
+    <row r="294" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B294" s="6">
         <v>64321</v>
       </c>
@@ -10203,10 +9317,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="295" spans="1:8">
-      <c r="A295" s="9">
-        <v>44988</v>
-      </c>
+    <row r="295" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B295" s="6">
         <v>64819</v>
       </c>
@@ -10229,10 +9340,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="296" spans="1:8">
-      <c r="A296" s="9">
-        <v>44988</v>
-      </c>
+    <row r="296" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B296" s="6">
         <v>65171</v>
       </c>
@@ -10255,10 +9363,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="297" spans="1:8">
-      <c r="A297" s="9">
-        <v>44988</v>
-      </c>
+    <row r="297" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B297" s="6">
         <v>65255</v>
       </c>
@@ -10281,7 +9386,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="302" spans="1:8">
+    <row r="302" spans="2:8" ht="13.5" x14ac:dyDescent="0.2">
       <c r="B302" s="1"/>
       <c r="F302" s="2"/>
       <c r="G302" s="3"/>
@@ -10294,6 +9399,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100963BF6C78482F94E9C3A8CBAE1AB6B06" ma:contentTypeVersion="18" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="859a2229eb1d12c7746815e94b49e62d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="95c80e47-662b-4bc0-a457-b879d3f3aba4" xmlns:ns3="7f019ab0-5ffe-43e1-b2f8-62bc369ebe4f" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="40415db81e42c57b7ee018001e89900f" ns2:_="" ns3:_="">
     <xsd:import namespace="95c80e47-662b-4bc0-a457-b879d3f3aba4"/>
@@ -10548,16 +9662,15 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{55482046-649C-48A1-B370-2C92212CADF5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{21E0C65F-3597-4AC8-AA07-17292E195C97}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -10574,12 +9687,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{55482046-649C-48A1-B370-2C92212CADF5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>